<commit_message>
Refactor structure of baselines
</commit_message>
<xml_diff>
--- a/_work/BaselineHeatMap.xlsx
+++ b/_work/BaselineHeatMap.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothydement/Google Drive/NCSU/3-Fall-2018/CSC-591-023/CodeSmellsClassifiers/_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6806F98-B026-1649-AE9F-C43531A7BA79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F1A744-FD85-D240-830B-981BC041EF7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{6CF25D03-8ECB-0B44-A74D-D4DF88305A38}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18600" windowHeight="17540" activeTab="1" xr2:uid="{6CF25D03-8ECB-0B44-A74D-D4DF88305A38}"/>
   </bookViews>
   <sheets>
-    <sheet name="Baseline" sheetId="1" r:id="rId1"/>
+    <sheet name="Baseline-All" sheetId="1" r:id="rId1"/>
+    <sheet name="Baseline-Med" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="32">
   <si>
     <t>1R</t>
   </si>
@@ -104,19 +105,46 @@
   </si>
   <si>
     <t>4/4</t>
+  </si>
+  <si>
+    <t>↑ Kappa (med)</t>
+  </si>
+  <si>
+    <t>↑ Acc (med)</t>
+  </si>
+  <si>
+    <t>↑ F-Score (med)</t>
+  </si>
+  <si>
+    <t>↑ Inform (med)</t>
+  </si>
+  <si>
+    <t>↓ Pct-DtH (med)</t>
+  </si>
+  <si>
+    <t>Top-Ranking</t>
+  </si>
+  <si>
+    <t>Bottom-Ranking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -261,147 +289,222 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -723,28 +826,28 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="10.83203125" style="7"/>
-    <col min="4" max="4" width="10.83203125" style="9"/>
-    <col min="5" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="6" width="10.83203125" style="9"/>
-    <col min="7" max="7" width="10.83203125" style="7"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
-    <col min="9" max="9" width="10.83203125" style="7"/>
-    <col min="10" max="10" width="10.83203125" style="9"/>
-    <col min="11" max="11" width="10.83203125" style="7"/>
-    <col min="12" max="12" width="10.83203125" style="9"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="10.83203125" style="8"/>
+    <col min="4" max="4" width="10.83203125" style="10"/>
+    <col min="5" max="5" width="10.83203125" style="8"/>
+    <col min="6" max="6" width="10.83203125" style="10"/>
+    <col min="7" max="7" width="10.83203125" style="8"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="10.83203125" style="8"/>
+    <col min="10" max="10" width="10.83203125" style="10"/>
+    <col min="11" max="11" width="10.83203125" style="8"/>
+    <col min="12" max="12" width="10.83203125" style="10"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+      <c r="A1" s="3"/>
       <c r="B1" s="17"/>
       <c r="C1" s="19" t="s">
         <v>5</v>
@@ -762,786 +865,786 @@
         <v>8</v>
       </c>
       <c r="J1" s="17"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="39" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="43">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="43">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="43">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I3" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="33">
+      <c r="I3" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="43">
         <v>0.19</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="12">
+      <c r="K3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="44">
         <v>0.49</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="45">
         <v>0.63</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="45">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="45">
         <v>0.3</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="21">
+      <c r="I4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="45">
         <v>0.25</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="44">
         <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="21">
+      <c r="C5" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="45">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="45">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="45">
         <v>0.09</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="45">
         <v>0.17</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="44">
         <v>0.42</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="C6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="45">
         <v>0.69</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="45">
         <v>0.53</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="45">
         <v>0.4</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="21">
+      <c r="I6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="45">
         <v>0.31</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="44">
         <v>0.41</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="39">
+        <v>17</v>
+      </c>
+      <c r="D7" s="46">
         <v>0.63</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="46">
         <v>0</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="46">
         <v>0.27</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="46">
         <v>0</v>
       </c>
-      <c r="K7" s="46" t="s">
+      <c r="K7" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="47">
         <v>0.71</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="33">
+      <c r="C8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="43">
         <v>0.96</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="43">
         <v>0.96</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="33">
+      <c r="G8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="43">
         <v>0.93</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="43">
         <v>0.93</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="44">
         <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="45">
         <v>0.96</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="45">
         <v>0.96</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="G9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="45">
         <v>0.92</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="45">
         <v>0.93</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="44">
         <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="21">
+      <c r="C10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="45">
         <v>0.88</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="45">
         <v>0.84</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="45">
         <v>0.75</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="45">
         <v>0.73</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="12">
-        <v>0.06</v>
+      <c r="K10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="44">
+        <v>0.19</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="45">
+        <v>0.96</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="45">
+        <v>0.95</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="45">
+        <v>0.92</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="45">
+        <v>0.91</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="44">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="21">
-        <v>0.96</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0.95</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="21">
-        <v>0.92</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="21">
-        <v>0.91</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="39">
+      <c r="D12" s="46">
         <v>0.76</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="46">
         <v>0.8</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="46">
         <v>0.5</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="46">
         <v>0.54</v>
       </c>
-      <c r="K12" s="46" t="s">
+      <c r="K12" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="47">
         <v>0.33</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="33">
+      <c r="C13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="43">
         <v>0.97</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="33">
+      <c r="E13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="43">
         <v>0.97</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="33">
+      <c r="G13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="43">
         <v>0.94</v>
       </c>
-      <c r="I13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="33">
+      <c r="I13" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="43">
         <v>0.94</v>
       </c>
-      <c r="K13" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="43">
+      <c r="K13" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="48">
         <v>0.04</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="45">
         <v>0.97</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="45">
         <v>0.97</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="45">
         <v>0.94</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="45">
         <v>0.94</v>
       </c>
-      <c r="K14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="12">
+      <c r="K14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="44">
         <v>0.04</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="45">
         <v>0.97</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="45">
         <v>0.97</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="45">
         <v>0.94</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="45">
         <v>0.94</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="12">
+      <c r="K15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="44">
         <v>0.04</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="21">
+      <c r="C16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="45">
         <v>1</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="21">
+      <c r="E16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="45">
         <v>1</v>
       </c>
-      <c r="G16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="21">
+      <c r="G16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="45">
         <v>1</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="21">
+      <c r="I16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="45">
         <v>1</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="46">
         <v>0.66</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="46">
         <v>0.42</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="46">
         <v>0.27</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="46">
         <v>0.27</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="K17" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="44">
+      <c r="L17" s="47">
         <v>0.52</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="43">
         <v>0.62</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="33">
+      <c r="E18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="43">
         <v>0.46</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="43">
         <v>0.2</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="45">
         <v>0.15</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L18" s="12">
+      <c r="K18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="44">
         <v>0.48</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="45">
         <v>0.64</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="45">
         <v>0.56000000000000005</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="45">
         <v>0.31</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="21">
+      <c r="I19" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="45">
         <v>0.24</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="44">
         <v>0.39</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="45">
         <v>0.7</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="45">
         <v>0.53</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="45">
         <v>0.36</v>
       </c>
-      <c r="I20" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="21">
+      <c r="I20" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="45">
         <v>0.32</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="12">
-        <v>0.42</v>
+      <c r="L20" s="44">
+        <v>0.43</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="45">
         <v>0.67</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="45">
         <v>0.53</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="45">
         <v>0.38</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="21">
+      <c r="I21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="45">
         <v>0.28000000000000003</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="44">
         <v>0.41</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="45">
         <v>0.59</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="45">
         <v>0.18</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="45">
         <v>0.18</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="45">
         <v>0.03</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="44">
         <v>0.64</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="10"/>
+    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1559,4 +1662,491 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292424F5-D988-DB43-BEDE-7EC511278674}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="49">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D2" s="60">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E2" s="49">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F2" s="56">
+        <v>0.19</v>
+      </c>
+      <c r="G2" s="57">
+        <v>0.49</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="54">
+        <v>0.63</v>
+      </c>
+      <c r="D3" s="59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E3" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="62">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="69"/>
+    </row>
+    <row r="4" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="59">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D4" s="59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.09</v>
+      </c>
+      <c r="F4" s="54">
+        <v>0.17</v>
+      </c>
+      <c r="G4" s="62">
+        <v>0.42</v>
+      </c>
+      <c r="I4" s="70"/>
+    </row>
+    <row r="5" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="59">
+        <v>0.69</v>
+      </c>
+      <c r="D5" s="59">
+        <v>0.53</v>
+      </c>
+      <c r="E5" s="59">
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="59">
+        <v>0.31</v>
+      </c>
+      <c r="G5" s="62">
+        <v>0.41</v>
+      </c>
+      <c r="I5" s="71"/>
+    </row>
+    <row r="6" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="55">
+        <v>0.63</v>
+      </c>
+      <c r="D6" s="50">
+        <v>0</v>
+      </c>
+      <c r="E6" s="61">
+        <v>0.27</v>
+      </c>
+      <c r="F6" s="50">
+        <v>0</v>
+      </c>
+      <c r="G6" s="53">
+        <v>0.71</v>
+      </c>
+      <c r="I6" s="72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="60">
+        <v>0.96</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0.96</v>
+      </c>
+      <c r="E7" s="60">
+        <v>0.93</v>
+      </c>
+      <c r="F7" s="60">
+        <v>0.93</v>
+      </c>
+      <c r="G7" s="62">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="59">
+        <v>0.96</v>
+      </c>
+      <c r="D8" s="59">
+        <v>0.96</v>
+      </c>
+      <c r="E8" s="59">
+        <v>0.92</v>
+      </c>
+      <c r="F8" s="59">
+        <v>0.93</v>
+      </c>
+      <c r="G8" s="62">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="54">
+        <v>0.88</v>
+      </c>
+      <c r="D9" s="51">
+        <v>0.84</v>
+      </c>
+      <c r="E9" s="54">
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="66">
+        <v>0.73</v>
+      </c>
+      <c r="G9" s="65">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="59">
+        <v>0.96</v>
+      </c>
+      <c r="D10" s="59">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="59">
+        <v>0.92</v>
+      </c>
+      <c r="F10" s="63">
+        <v>0.91</v>
+      </c>
+      <c r="G10" s="64">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="50">
+        <v>0.76</v>
+      </c>
+      <c r="D11" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="E11" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="50">
+        <v>0.54</v>
+      </c>
+      <c r="G11" s="53">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="56">
+        <v>0.97</v>
+      </c>
+      <c r="D12" s="56">
+        <v>0.97</v>
+      </c>
+      <c r="E12" s="56">
+        <v>0.94</v>
+      </c>
+      <c r="F12" s="56">
+        <v>0.94</v>
+      </c>
+      <c r="G12" s="58">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="54">
+        <v>0.97</v>
+      </c>
+      <c r="D13" s="54">
+        <v>0.97</v>
+      </c>
+      <c r="E13" s="54">
+        <v>0.94</v>
+      </c>
+      <c r="F13" s="54">
+        <v>0.94</v>
+      </c>
+      <c r="G13" s="57">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="54">
+        <v>0.97</v>
+      </c>
+      <c r="D14" s="54">
+        <v>0.97</v>
+      </c>
+      <c r="E14" s="54">
+        <v>0.94</v>
+      </c>
+      <c r="F14" s="54">
+        <v>0.94</v>
+      </c>
+      <c r="G14" s="57">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="59">
+        <v>1</v>
+      </c>
+      <c r="D15" s="59">
+        <v>1</v>
+      </c>
+      <c r="E15" s="59">
+        <v>1</v>
+      </c>
+      <c r="F15" s="59">
+        <v>1</v>
+      </c>
+      <c r="G15" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="50">
+        <v>0.66</v>
+      </c>
+      <c r="D16" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="E16" s="50">
+        <v>0.27</v>
+      </c>
+      <c r="F16" s="50">
+        <v>0.27</v>
+      </c>
+      <c r="G16" s="53">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="49">
+        <v>0.62</v>
+      </c>
+      <c r="D17" s="56">
+        <v>0.46</v>
+      </c>
+      <c r="E17" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="54">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="57">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="51">
+        <v>0.64</v>
+      </c>
+      <c r="D18" s="59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E18" s="51">
+        <v>0.31</v>
+      </c>
+      <c r="F18" s="59">
+        <v>0.24</v>
+      </c>
+      <c r="G18" s="62">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="59">
+        <v>0.7</v>
+      </c>
+      <c r="D19" s="59">
+        <v>0.53</v>
+      </c>
+      <c r="E19" s="59">
+        <v>0.36</v>
+      </c>
+      <c r="F19" s="59">
+        <v>0.32</v>
+      </c>
+      <c r="G19" s="62">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="59">
+        <v>0.67</v>
+      </c>
+      <c r="D20" s="59">
+        <v>0.53</v>
+      </c>
+      <c r="E20" s="59">
+        <v>0.38</v>
+      </c>
+      <c r="F20" s="59">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G20" s="62">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="51">
+        <v>0.59</v>
+      </c>
+      <c r="D21" s="51">
+        <v>0.18</v>
+      </c>
+      <c r="E21" s="51">
+        <v>0.18</v>
+      </c>
+      <c r="F21" s="51">
+        <v>0.03</v>
+      </c>
+      <c r="G21" s="52">
+        <v>0.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>